<commit_message>
Tweaked text font, miscellaneous bug fixes
</commit_message>
<xml_diff>
--- a/XMP/XMPtoFilterMapping.xlsx
+++ b/XMP/XMPtoFilterMapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philprice95/Documents/iOS/phixer/XMP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E511FBA-F143-B146-9136-79D268760AD8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A0FBEF-5577-A548-BAB5-81C1235EE1EB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16880" yWindow="6440" windowWidth="34320" windowHeight="20760" xr2:uid="{4C672D77-E69B-514D-8556-8F808505B8EF}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1497" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1522" uniqueCount="515">
   <si>
     <t>Property</t>
   </si>
@@ -1561,6 +1561,21 @@
   </si>
   <si>
     <t>inputTint</t>
+  </si>
+  <si>
+    <t>CINoiseReduction</t>
+  </si>
+  <si>
+    <t>GrainFilter</t>
+  </si>
+  <si>
+    <t>HSV</t>
+  </si>
+  <si>
+    <t>SplitToningFilter</t>
+  </si>
+  <si>
+    <t>RGBChannelToneCurve</t>
   </si>
 </sst>
 </file>
@@ -1964,8 +1979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5B5CED5-45A2-354E-B64A-518AA8F25FF5}">
   <dimension ref="A1:H229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28:C36"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
@@ -2309,14 +2324,14 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>490</v>
+      <c r="A15" s="2" t="s">
+        <v>510</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>103</v>
+        <v>40</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>103</v>
+        <v>41</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>23</v>
@@ -2328,18 +2343,18 @@
         <v>10</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>104</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>492</v>
+      <c r="A16" s="2" t="s">
+        <v>510</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>182</v>
+        <v>297</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>183</v>
+        <v>298</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>23</v>
@@ -2355,14 +2370,14 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>492</v>
+      <c r="A17" s="2" t="s">
+        <v>510</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>184</v>
+        <v>352</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>185</v>
+        <v>353</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>23</v>
@@ -2379,13 +2394,13 @@
     </row>
     <row r="18" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>186</v>
+        <v>103</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>187</v>
+        <v>103</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>23</v>
@@ -2397,7 +2412,7 @@
         <v>10</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>131</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="19" x14ac:dyDescent="0.25">
@@ -2405,10 +2420,10 @@
         <v>492</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>23</v>
@@ -2428,10 +2443,10 @@
         <v>492</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>23</v>
@@ -2451,10 +2466,10 @@
         <v>492</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>23</v>
@@ -2474,10 +2489,10 @@
         <v>492</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>23</v>
@@ -2497,13 +2512,13 @@
         <v>492</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>109</v>
+        <v>190</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>110</v>
+        <v>191</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>111</v>
+        <v>23</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>9</v>
@@ -2512,7 +2527,7 @@
         <v>10</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="19" x14ac:dyDescent="0.25">
@@ -2520,13 +2535,13 @@
         <v>492</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>113</v>
+        <v>192</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>114</v>
+        <v>193</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>115</v>
+        <v>23</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>9</v>
@@ -2535,7 +2550,7 @@
         <v>10</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>116</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="19" x14ac:dyDescent="0.25">
@@ -2543,13 +2558,13 @@
         <v>492</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>322</v>
+        <v>194</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>323</v>
+        <v>195</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>9</v>
@@ -2558,7 +2573,7 @@
         <v>10</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>324</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="19" x14ac:dyDescent="0.25">
@@ -2566,10 +2581,10 @@
         <v>492</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>331</v>
+        <v>109</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>332</v>
+        <v>110</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>111</v>
@@ -2586,16 +2601,16 @@
     </row>
     <row r="27" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>228</v>
+        <v>113</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>228</v>
+        <v>114</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>23</v>
+        <v>115</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>9</v>
@@ -2604,44 +2619,44 @@
         <v>10</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>450</v>
+        <v>322</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>450</v>
+        <v>323</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>428</v>
+        <v>10</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>131</v>
+        <v>324</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>253</v>
+        <v>331</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>254</v>
+        <v>332</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>23</v>
+        <v>111</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>9</v>
@@ -2650,18 +2665,18 @@
         <v>10</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>257</v>
+        <v>228</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>258</v>
+        <v>228</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>23</v>
@@ -2681,19 +2696,19 @@
         <v>488</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>255</v>
+        <v>450</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>256</v>
+        <v>450</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>10</v>
+        <v>428</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>131</v>
@@ -2704,10 +2719,10 @@
         <v>488</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>23</v>
@@ -2727,10 +2742,10 @@
         <v>488</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>23</v>
@@ -2750,19 +2765,19 @@
         <v>488</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>431</v>
+        <v>255</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>431</v>
+        <v>256</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>428</v>
+        <v>10</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>131</v>
@@ -2773,10 +2788,10 @@
         <v>488</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>119</v>
+        <v>259</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>120</v>
+        <v>260</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>23</v>
@@ -2788,7 +2803,7 @@
         <v>10</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="19" x14ac:dyDescent="0.25">
@@ -2796,10 +2811,10 @@
         <v>488</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>122</v>
+        <v>261</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>123</v>
+        <v>262</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>23</v>
@@ -2811,178 +2826,169 @@
         <v>10</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C40" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D40" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="E37" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+      <c r="E40" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>487</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C41" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D41" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="E38" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="E41" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C42" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D42" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E39" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H39" s="3" t="s">
+      <c r="E42" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H42" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+    <row r="43" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C43" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D43" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="E40" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>503</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>503</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>503</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>197</v>
-      </c>
       <c r="E43" s="3" t="s">
         <v>23</v>
       </c>
@@ -2997,17 +3003,14 @@
       </c>
     </row>
     <row r="44" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>480</v>
+      <c r="A44" s="2" t="s">
+        <v>511</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>21</v>
+        <v>299</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>22</v>
+        <v>300</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>23</v>
@@ -3019,21 +3022,18 @@
         <v>10</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>24</v>
+        <v>131</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>480</v>
+      <c r="A45" s="2" t="s">
+        <v>511</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>25</v>
+        <v>303</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>26</v>
+        <v>303</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>23</v>
@@ -3045,21 +3045,18 @@
         <v>10</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>27</v>
+        <v>131</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>480</v>
+      <c r="A46" s="2" t="s">
+        <v>511</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>148</v>
+        <v>301</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>149</v>
+        <v>302</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>23</v>
@@ -3075,17 +3072,14 @@
       </c>
     </row>
     <row r="47" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>480</v>
+      <c r="A47" s="2" t="s">
+        <v>512</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>168</v>
+        <v>237</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>169</v>
+        <v>238</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>23</v>
@@ -3101,17 +3095,14 @@
       </c>
     </row>
     <row r="48" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>480</v>
+      <c r="A48" s="2" t="s">
+        <v>512</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>198</v>
+        <v>239</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>199</v>
+        <v>240</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>23</v>
@@ -3127,17 +3118,14 @@
       </c>
     </row>
     <row r="49" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>501</v>
+      <c r="A49" s="2" t="s">
+        <v>512</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>72</v>
+        <v>235</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>73</v>
+        <v>236</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>23</v>
@@ -3149,21 +3137,18 @@
         <v>10</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>74</v>
+        <v>131</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>501</v>
+      <c r="A50" s="2" t="s">
+        <v>512</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>75</v>
+        <v>243</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>76</v>
+        <v>244</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>23</v>
@@ -3175,21 +3160,18 @@
         <v>10</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>77</v>
+        <v>131</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>501</v>
+      <c r="A51" s="2" t="s">
+        <v>512</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>150</v>
+        <v>231</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>151</v>
+        <v>232</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>23</v>
@@ -3205,17 +3187,14 @@
       </c>
     </row>
     <row r="52" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>501</v>
+      <c r="A52" s="2" t="s">
+        <v>512</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>170</v>
+        <v>241</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>171</v>
+        <v>242</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>23</v>
@@ -3231,17 +3210,14 @@
       </c>
     </row>
     <row r="53" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>501</v>
+      <c r="A53" s="2" t="s">
+        <v>512</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>200</v>
+        <v>229</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>201</v>
+        <v>230</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>23</v>
@@ -3257,17 +3233,14 @@
       </c>
     </row>
     <row r="54" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>504</v>
+      <c r="A54" s="2" t="s">
+        <v>512</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>152</v>
+        <v>233</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>153</v>
+        <v>234</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>23</v>
@@ -3287,13 +3260,13 @@
         <v>479</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>173</v>
+        <v>147</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>23</v>
@@ -3313,13 +3286,13 @@
         <v>479</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>202</v>
+        <v>166</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>203</v>
+        <v>167</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>23</v>
@@ -3339,13 +3312,13 @@
         <v>479</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>154</v>
+        <v>196</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>155</v>
+        <v>197</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>23</v>
@@ -3365,13 +3338,13 @@
         <v>479</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>505</v>
+        <v>480</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>174</v>
+        <v>21</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>175</v>
+        <v>22</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>23</v>
@@ -3383,7 +3356,7 @@
         <v>10</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>131</v>
+        <v>24</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="19" x14ac:dyDescent="0.25">
@@ -3391,13 +3364,13 @@
         <v>479</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>505</v>
+        <v>480</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>204</v>
+        <v>25</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>205</v>
+        <v>26</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>23</v>
@@ -3409,7 +3382,7 @@
         <v>10</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>131</v>
+        <v>27</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="19" x14ac:dyDescent="0.25">
@@ -3417,13 +3390,13 @@
         <v>479</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>506</v>
+        <v>480</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>23</v>
@@ -3443,13 +3416,13 @@
         <v>479</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>506</v>
+        <v>480</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>23</v>
@@ -3469,13 +3442,13 @@
         <v>479</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>506</v>
+        <v>480</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>23</v>
@@ -3495,13 +3468,13 @@
         <v>479</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>158</v>
+        <v>72</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>159</v>
+        <v>73</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>23</v>
@@ -3513,7 +3486,7 @@
         <v>10</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>131</v>
+        <v>74</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="19" x14ac:dyDescent="0.25">
@@ -3521,13 +3494,13 @@
         <v>479</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>178</v>
+        <v>75</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>179</v>
+        <v>76</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>23</v>
@@ -3539,7 +3512,7 @@
         <v>10</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>131</v>
+        <v>77</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="19" x14ac:dyDescent="0.25">
@@ -3547,13 +3520,13 @@
         <v>479</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>91</v>
+        <v>151</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>23</v>
@@ -3565,7 +3538,7 @@
         <v>10</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>92</v>
+        <v>131</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="19" x14ac:dyDescent="0.25">
@@ -3573,13 +3546,13 @@
         <v>479</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>93</v>
+        <v>170</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>94</v>
+        <v>171</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>23</v>
@@ -3591,7 +3564,7 @@
         <v>10</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>95</v>
+        <v>131</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="19" x14ac:dyDescent="0.25">
@@ -3599,13 +3572,13 @@
         <v>479</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>23</v>
@@ -3625,13 +3598,13 @@
         <v>479</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>23</v>
@@ -3651,13 +3624,13 @@
         <v>479</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>23</v>
@@ -3677,13 +3650,13 @@
         <v>479</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>23</v>
@@ -3700,16 +3673,16 @@
     </row>
     <row r="71" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>497</v>
+        <v>505</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>96</v>
+        <v>154</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>96</v>
+        <v>155</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>23</v>
@@ -3721,21 +3694,21 @@
         <v>10</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>97</v>
+        <v>131</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>493</v>
+        <v>479</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>499</v>
+        <v>505</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>212</v>
+        <v>174</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>213</v>
+        <v>175</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>23</v>
@@ -3752,19 +3725,19 @@
     </row>
     <row r="73" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>493</v>
+        <v>479</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>498</v>
+        <v>505</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="F73" s="3" t="s">
         <v>9</v>
@@ -3777,17 +3750,17 @@
       </c>
     </row>
     <row r="74" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
-        <v>493</v>
+      <c r="A74" s="1" t="s">
+        <v>479</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>500</v>
+        <v>506</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>214</v>
+        <v>156</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>215</v>
+        <v>157</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>23</v>
@@ -3804,16 +3777,16 @@
     </row>
     <row r="75" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>491</v>
+        <v>479</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>163</v>
+        <v>177</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>23</v>
@@ -3830,16 +3803,16 @@
     </row>
     <row r="76" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>491</v>
+        <v>479</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>105</v>
+        <v>206</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>105</v>
+        <v>207</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>23</v>
@@ -3851,21 +3824,21 @@
         <v>10</v>
       </c>
       <c r="H76" s="3" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>491</v>
+        <v>479</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>509</v>
+        <v>502</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>23</v>
@@ -3882,16 +3855,16 @@
     </row>
     <row r="78" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>491</v>
+        <v>479</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>509</v>
+        <v>502</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>107</v>
+        <v>178</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>107</v>
+        <v>179</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>23</v>
@@ -3903,538 +3876,655 @@
         <v>10</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F79" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G79" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H79" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G80" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H80" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F81" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G81" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H81" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F82" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H82" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G83" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H83" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H84" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H85" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F86" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H86" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F87" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H87" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F88" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H88" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F89" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H89" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F90" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H90" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F91" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G91" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H91" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F92" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H92" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F93" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G93" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H93" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F94" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G94" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H94" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F95" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G95" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H95" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F96" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H96" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F97" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G97" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H97" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F98" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G98" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H98" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F99" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G99" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H99" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="C79" s="3" t="s">
+      <c r="B100" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="E100" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F100" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G100" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H100" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E101" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F101" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G101" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H101" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F102" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G102" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H102" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E103" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F103" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G103" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H103" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="C104" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D79" s="3" t="s">
+      <c r="D104" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="E79" s="3" t="s">
+      <c r="E104" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="F79" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G79" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H79" s="3" t="s">
+      <c r="F104" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G104" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H104" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="C80" s="3" t="s">
+    <row r="105" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="C105" s="3" t="s">
         <v>460</v>
       </c>
-      <c r="D80" s="3" t="s">
+      <c r="D105" s="3" t="s">
         <v>460</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F80" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G80" s="3" t="s">
-        <v>428</v>
-      </c>
-      <c r="H80" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="81" spans="3:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="C81" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E81" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F81" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G81" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H81" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="82" spans="3:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="C82" s="3" t="s">
-        <v>449</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>449</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F82" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G82" s="3" t="s">
-        <v>428</v>
-      </c>
-      <c r="H82" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="83" spans="3:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="C83" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="E83" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F83" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G83" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H83" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="84" spans="3:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="C84" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="E84" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F84" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G84" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H84" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="85" spans="3:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="C85" s="3" t="s">
-        <v>447</v>
-      </c>
-      <c r="D85" s="3" t="s">
-        <v>447</v>
-      </c>
-      <c r="E85" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F85" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G85" s="3" t="s">
-        <v>428</v>
-      </c>
-      <c r="H85" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="86" spans="3:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="C86" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D86" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E86" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F86" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G86" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H86" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="87" spans="3:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="C87" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="D87" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="E87" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F87" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G87" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H87" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="88" spans="3:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="C88" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="D88" s="3" t="s">
-        <v>462</v>
-      </c>
-      <c r="E88" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F88" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G88" s="3" t="s">
-        <v>428</v>
-      </c>
-      <c r="H88" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="89" spans="3:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="C89" s="3" t="s">
-        <v>433</v>
-      </c>
-      <c r="D89" s="3" t="s">
-        <v>434</v>
-      </c>
-      <c r="E89" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F89" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G89" s="3" t="s">
-        <v>428</v>
-      </c>
-      <c r="H89" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="90" spans="3:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="C90" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D90" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E90" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F90" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G90" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H90" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="91" spans="3:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="C91" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D91" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E91" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F91" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G91" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H91" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="92" spans="3:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="C92" s="3" t="s">
-        <v>422</v>
-      </c>
-      <c r="D92" s="3" t="s">
-        <v>422</v>
-      </c>
-      <c r="E92" s="3" t="s">
-        <v>422</v>
-      </c>
-      <c r="F92" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G92" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H92" s="3" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="93" spans="3:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="C93" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D93" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E93" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F93" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G93" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H93" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="94" spans="3:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="C94" s="3" t="s">
-        <v>297</v>
-      </c>
-      <c r="D94" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="E94" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F94" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G94" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H94" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="95" spans="3:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="C95" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="D95" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="E95" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F95" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G95" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H95" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="96" spans="3:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="C96" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="D96" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="E96" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F96" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G96" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H96" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="97" spans="3:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="C97" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="D97" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="E97" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F97" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G97" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H97" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="98" spans="3:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="C98" s="3" t="s">
-        <v>425</v>
-      </c>
-      <c r="D98" s="3" t="s">
-        <v>425</v>
-      </c>
-      <c r="E98" s="3" t="s">
-        <v>425</v>
-      </c>
-      <c r="F98" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G98" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H98" s="3" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="99" spans="3:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="C99" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D99" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E99" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F99" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G99" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H99" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="100" spans="3:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="C100" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D100" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E100" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F100" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G100" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H100" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="101" spans="3:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="C101" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="D101" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="E101" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F101" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G101" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H101" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="102" spans="3:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="C102" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D102" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E102" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F102" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G102" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H102" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="103" spans="3:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="C103" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D103" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E103" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F103" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G103" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H103" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="104" spans="3:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="C104" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D104" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E104" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F104" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G104" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H104" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="105" spans="3:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="C105" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D105" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>47</v>
@@ -4443,21 +4533,21 @@
         <v>9</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>10</v>
+        <v>428</v>
       </c>
       <c r="H105" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="106" spans="3:8" ht="19" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C106" s="3" t="s">
-        <v>251</v>
+        <v>129</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>252</v>
+        <v>130</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="F106" s="3" t="s">
         <v>9</v>
@@ -4469,95 +4559,95 @@
         <v>131</v>
       </c>
     </row>
-    <row r="107" spans="3:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C107" s="3" t="s">
-        <v>67</v>
+        <v>449</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>68</v>
+        <v>449</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="F107" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>10</v>
+        <v>428</v>
       </c>
       <c r="H107" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="108" spans="3:8" ht="19" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C108" s="3" t="s">
-        <v>61</v>
+        <v>304</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>62</v>
+        <v>305</v>
       </c>
       <c r="E108" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F108" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G108" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H108" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="C109" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="E109" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F109" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G109" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H109" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="C110" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="E110" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F108" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G108" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H108" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="109" spans="3:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="C109" s="3" t="s">
-        <v>435</v>
-      </c>
-      <c r="D109" s="3" t="s">
-        <v>435</v>
-      </c>
-      <c r="E109" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="F109" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G109" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H109" s="3" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="110" spans="3:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="C110" s="3" t="s">
-        <v>404</v>
-      </c>
-      <c r="D110" s="3" t="s">
-        <v>405</v>
-      </c>
-      <c r="E110" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="F110" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G110" s="3" t="s">
-        <v>10</v>
+        <v>428</v>
       </c>
       <c r="H110" s="3" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="111" spans="3:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C111" s="3" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>403</v>
+        <v>31</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="F111" s="3" t="s">
         <v>9</v>
@@ -4566,18 +4656,18 @@
         <v>10</v>
       </c>
       <c r="H111" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="112" spans="3:8" ht="19" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C112" s="3" t="s">
-        <v>408</v>
+        <v>136</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>409</v>
+        <v>137</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="F112" s="3" t="s">
         <v>9</v>
@@ -4591,19 +4681,19 @@
     </row>
     <row r="113" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C113" s="3" t="s">
-        <v>406</v>
+        <v>461</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>407</v>
+        <v>462</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="F113" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G113" s="3" t="s">
-        <v>10</v>
+        <v>428</v>
       </c>
       <c r="H113" s="3" t="s">
         <v>131</v>
@@ -4611,19 +4701,19 @@
     </row>
     <row r="114" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C114" s="3" t="s">
-        <v>141</v>
+        <v>433</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>141</v>
+        <v>434</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="F114" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>10</v>
+        <v>428</v>
       </c>
       <c r="H114" s="3" t="s">
         <v>131</v>
@@ -4631,10 +4721,10 @@
     </row>
     <row r="115" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C115" s="3" t="s">
-        <v>345</v>
+        <v>34</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>346</v>
+        <v>35</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>23</v>
@@ -4646,15 +4736,15 @@
         <v>10</v>
       </c>
       <c r="H115" s="3" t="s">
-        <v>131</v>
+        <v>36</v>
       </c>
     </row>
     <row r="116" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C116" s="3" t="s">
-        <v>349</v>
+        <v>37</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>350</v>
+        <v>38</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>23</v>
@@ -4666,18 +4756,18 @@
         <v>10</v>
       </c>
       <c r="H116" s="3" t="s">
-        <v>131</v>
+        <v>39</v>
       </c>
     </row>
     <row r="117" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C117" s="3" t="s">
-        <v>347</v>
+        <v>422</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>348</v>
+        <v>422</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>23</v>
+        <v>422</v>
       </c>
       <c r="F117" s="3" t="s">
         <v>9</v>
@@ -4686,18 +4776,18 @@
         <v>10</v>
       </c>
       <c r="H117" s="3" t="s">
-        <v>131</v>
+        <v>423</v>
       </c>
     </row>
     <row r="118" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C118" s="3" t="s">
-        <v>339</v>
+        <v>132</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>340</v>
+        <v>132</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="F118" s="3" t="s">
         <v>9</v>
@@ -4711,13 +4801,13 @@
     </row>
     <row r="119" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C119" s="3" t="s">
-        <v>343</v>
+        <v>139</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>344</v>
+        <v>140</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="F119" s="3" t="s">
         <v>9</v>
@@ -4731,13 +4821,13 @@
     </row>
     <row r="120" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C120" s="3" t="s">
-        <v>341</v>
+        <v>425</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>342</v>
+        <v>425</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>23</v>
+        <v>425</v>
       </c>
       <c r="F120" s="3" t="s">
         <v>9</v>
@@ -4746,18 +4836,18 @@
         <v>10</v>
       </c>
       <c r="H120" s="3" t="s">
-        <v>131</v>
+        <v>426</v>
       </c>
     </row>
     <row r="121" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C121" s="3" t="s">
-        <v>410</v>
+        <v>58</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>411</v>
+        <v>59</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="F121" s="3" t="s">
         <v>9</v>
@@ -4766,15 +4856,15 @@
         <v>10</v>
       </c>
       <c r="H121" s="3" t="s">
-        <v>131</v>
+        <v>60</v>
       </c>
     </row>
     <row r="122" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C122" s="3" t="s">
-        <v>452</v>
+        <v>52</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>452</v>
+        <v>53</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>47</v>
@@ -4783,27 +4873,27 @@
         <v>9</v>
       </c>
       <c r="G122" s="3" t="s">
-        <v>428</v>
+        <v>10</v>
       </c>
       <c r="H122" s="3" t="s">
-        <v>131</v>
+        <v>54</v>
       </c>
     </row>
     <row r="123" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C123" s="3" t="s">
-        <v>452</v>
+        <v>291</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>452</v>
+        <v>292</v>
       </c>
       <c r="E123" s="3" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="F123" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G123" s="3" t="s">
-        <v>428</v>
+        <v>10</v>
       </c>
       <c r="H123" s="3" t="s">
         <v>131</v>
@@ -4811,13 +4901,13 @@
     </row>
     <row r="124" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C124" s="3" t="s">
-        <v>142</v>
+        <v>64</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>143</v>
+        <v>65</v>
       </c>
       <c r="E124" s="3" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="F124" s="3" t="s">
         <v>9</v>
@@ -4826,35 +4916,35 @@
         <v>10</v>
       </c>
       <c r="H124" s="3" t="s">
-        <v>131</v>
+        <v>66</v>
       </c>
     </row>
     <row r="125" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C125" s="3" t="s">
-        <v>453</v>
+        <v>49</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>453</v>
+        <v>50</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="F125" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G125" s="3" t="s">
-        <v>428</v>
+        <v>10</v>
       </c>
       <c r="H125" s="3" t="s">
-        <v>131</v>
+        <v>51</v>
       </c>
     </row>
     <row r="126" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C126" s="3" t="s">
-        <v>432</v>
+        <v>55</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>432</v>
+        <v>56</v>
       </c>
       <c r="E126" s="3" t="s">
         <v>47</v>
@@ -4863,18 +4953,18 @@
         <v>9</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>428</v>
+        <v>10</v>
       </c>
       <c r="H126" s="3" t="s">
-        <v>131</v>
+        <v>57</v>
       </c>
     </row>
     <row r="127" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C127" s="3" t="s">
-        <v>441</v>
+        <v>45</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>442</v>
+        <v>46</v>
       </c>
       <c r="E127" s="3" t="s">
         <v>47</v>
@@ -4883,27 +4973,27 @@
         <v>9</v>
       </c>
       <c r="G127" s="3" t="s">
-        <v>428</v>
+        <v>10</v>
       </c>
       <c r="H127" s="3" t="s">
-        <v>131</v>
+        <v>48</v>
       </c>
     </row>
     <row r="128" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C128" s="3" t="s">
-        <v>443</v>
+        <v>251</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>444</v>
+        <v>252</v>
       </c>
       <c r="E128" s="3" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="F128" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G128" s="3" t="s">
-        <v>428</v>
+        <v>10</v>
       </c>
       <c r="H128" s="3" t="s">
         <v>131</v>
@@ -4911,10 +5001,10 @@
     </row>
     <row r="129" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C129" s="3" t="s">
-        <v>299</v>
+        <v>67</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>300</v>
+        <v>68</v>
       </c>
       <c r="E129" s="3" t="s">
         <v>23</v>
@@ -4926,18 +5016,18 @@
         <v>10</v>
       </c>
       <c r="H129" s="3" t="s">
-        <v>131</v>
+        <v>69</v>
       </c>
     </row>
     <row r="130" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C130" s="3" t="s">
-        <v>303</v>
+        <v>61</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>303</v>
+        <v>62</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="F130" s="3" t="s">
         <v>9</v>
@@ -4946,18 +5036,18 @@
         <v>10</v>
       </c>
       <c r="H130" s="3" t="s">
-        <v>131</v>
+        <v>63</v>
       </c>
     </row>
     <row r="131" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C131" s="3" t="s">
-        <v>301</v>
+        <v>435</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>302</v>
+        <v>435</v>
       </c>
       <c r="E131" s="3" t="s">
-        <v>23</v>
+        <v>111</v>
       </c>
       <c r="F131" s="3" t="s">
         <v>9</v>
@@ -4966,18 +5056,18 @@
         <v>10</v>
       </c>
       <c r="H131" s="3" t="s">
-        <v>131</v>
+        <v>436</v>
       </c>
     </row>
     <row r="132" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C132" s="3" t="s">
-        <v>237</v>
+        <v>404</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>238</v>
+        <v>405</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="F132" s="3" t="s">
         <v>9</v>
@@ -4991,13 +5081,13 @@
     </row>
     <row r="133" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C133" s="3" t="s">
-        <v>239</v>
+        <v>402</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>240</v>
+        <v>403</v>
       </c>
       <c r="E133" s="3" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="F133" s="3" t="s">
         <v>9</v>
@@ -5011,13 +5101,13 @@
     </row>
     <row r="134" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C134" s="3" t="s">
-        <v>235</v>
+        <v>408</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>236</v>
+        <v>409</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="F134" s="3" t="s">
         <v>9</v>
@@ -5031,13 +5121,13 @@
     </row>
     <row r="135" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C135" s="3" t="s">
-        <v>243</v>
+        <v>406</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>244</v>
+        <v>407</v>
       </c>
       <c r="E135" s="3" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="F135" s="3" t="s">
         <v>9</v>
@@ -5051,10 +5141,10 @@
     </row>
     <row r="136" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C136" s="3" t="s">
-        <v>231</v>
+        <v>141</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>232</v>
+        <v>141</v>
       </c>
       <c r="E136" s="3" t="s">
         <v>23</v>
@@ -5071,10 +5161,10 @@
     </row>
     <row r="137" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C137" s="3" t="s">
-        <v>241</v>
+        <v>345</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>242</v>
+        <v>346</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>23</v>
@@ -5091,10 +5181,10 @@
     </row>
     <row r="138" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C138" s="3" t="s">
-        <v>229</v>
+        <v>349</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>230</v>
+        <v>350</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>23</v>
@@ -5111,10 +5201,10 @@
     </row>
     <row r="139" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C139" s="3" t="s">
-        <v>233</v>
+        <v>347</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>234</v>
+        <v>348</v>
       </c>
       <c r="E139" s="3" t="s">
         <v>23</v>
@@ -5131,13 +5221,13 @@
     </row>
     <row r="140" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C140" s="3" t="s">
-        <v>78</v>
+        <v>339</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>79</v>
+        <v>340</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="F140" s="3" t="s">
         <v>9</v>
@@ -5146,18 +5236,18 @@
         <v>10</v>
       </c>
       <c r="H140" s="3" t="s">
-        <v>80</v>
+        <v>131</v>
       </c>
     </row>
     <row r="141" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C141" s="3" t="s">
-        <v>81</v>
+        <v>343</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>82</v>
+        <v>344</v>
       </c>
       <c r="E141" s="3" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="F141" s="3" t="s">
         <v>9</v>
@@ -5166,18 +5256,18 @@
         <v>10</v>
       </c>
       <c r="H141" s="3" t="s">
-        <v>83</v>
+        <v>131</v>
       </c>
     </row>
     <row r="142" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C142" s="3" t="s">
-        <v>418</v>
+        <v>341</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>419</v>
+        <v>342</v>
       </c>
       <c r="E142" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F142" s="3" t="s">
         <v>9</v>
@@ -5191,19 +5281,19 @@
     </row>
     <row r="143" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C143" s="3" t="s">
-        <v>446</v>
+        <v>410</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>446</v>
+        <v>411</v>
       </c>
       <c r="E143" s="3" t="s">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="F143" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G143" s="3" t="s">
-        <v>428</v>
+        <v>10</v>
       </c>
       <c r="H143" s="3" t="s">
         <v>131</v>
@@ -5211,19 +5301,19 @@
     </row>
     <row r="144" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C144" s="3" t="s">
-        <v>281</v>
+        <v>452</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>282</v>
+        <v>452</v>
       </c>
       <c r="E144" s="3" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="F144" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G144" s="3" t="s">
-        <v>10</v>
+        <v>428</v>
       </c>
       <c r="H144" s="3" t="s">
         <v>131</v>
@@ -5231,19 +5321,19 @@
     </row>
     <row r="145" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C145" s="3" t="s">
-        <v>277</v>
+        <v>452</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>278</v>
+        <v>452</v>
       </c>
       <c r="E145" s="3" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="F145" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G145" s="3" t="s">
-        <v>10</v>
+        <v>428</v>
       </c>
       <c r="H145" s="3" t="s">
         <v>131</v>
@@ -5251,13 +5341,13 @@
     </row>
     <row r="146" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C146" s="3" t="s">
-        <v>273</v>
+        <v>142</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>274</v>
+        <v>143</v>
       </c>
       <c r="E146" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F146" s="3" t="s">
         <v>9</v>
@@ -5271,19 +5361,19 @@
     </row>
     <row r="147" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C147" s="3" t="s">
-        <v>275</v>
+        <v>453</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>276</v>
+        <v>453</v>
       </c>
       <c r="E147" s="3" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="F147" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G147" s="3" t="s">
-        <v>10</v>
+        <v>428</v>
       </c>
       <c r="H147" s="3" t="s">
         <v>131</v>
@@ -5291,19 +5381,19 @@
     </row>
     <row r="148" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C148" s="3" t="s">
-        <v>265</v>
+        <v>432</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>266</v>
+        <v>432</v>
       </c>
       <c r="E148" s="3" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="F148" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G148" s="3" t="s">
-        <v>10</v>
+        <v>428</v>
       </c>
       <c r="H148" s="3" t="s">
         <v>131</v>
@@ -5311,19 +5401,19 @@
     </row>
     <row r="149" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C149" s="3" t="s">
-        <v>271</v>
+        <v>441</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>272</v>
+        <v>442</v>
       </c>
       <c r="E149" s="3" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="F149" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G149" s="3" t="s">
-        <v>10</v>
+        <v>428</v>
       </c>
       <c r="H149" s="3" t="s">
         <v>131</v>
@@ -5331,19 +5421,19 @@
     </row>
     <row r="150" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C150" s="3" t="s">
-        <v>390</v>
+        <v>443</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>391</v>
+        <v>444</v>
       </c>
       <c r="E150" s="3" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="F150" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G150" s="3" t="s">
-        <v>10</v>
+        <v>428</v>
       </c>
       <c r="H150" s="3" t="s">
         <v>131</v>
@@ -5351,13 +5441,13 @@
     </row>
     <row r="151" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C151" s="3" t="s">
-        <v>386</v>
+        <v>78</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>387</v>
+        <v>79</v>
       </c>
       <c r="E151" s="3" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="F151" s="3" t="s">
         <v>9</v>
@@ -5366,18 +5456,18 @@
         <v>10</v>
       </c>
       <c r="H151" s="3" t="s">
-        <v>131</v>
+        <v>80</v>
       </c>
     </row>
     <row r="152" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C152" s="3" t="s">
-        <v>388</v>
+        <v>81</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>389</v>
+        <v>82</v>
       </c>
       <c r="E152" s="3" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="F152" s="3" t="s">
         <v>9</v>
@@ -5386,18 +5476,18 @@
         <v>10</v>
       </c>
       <c r="H152" s="3" t="s">
-        <v>131</v>
+        <v>83</v>
       </c>
     </row>
     <row r="153" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C153" s="3" t="s">
-        <v>398</v>
+        <v>418</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>399</v>
+        <v>419</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="F153" s="3" t="s">
         <v>9</v>
@@ -5411,19 +5501,19 @@
     </row>
     <row r="154" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C154" s="3" t="s">
-        <v>394</v>
+        <v>446</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>395</v>
+        <v>446</v>
       </c>
       <c r="E154" s="3" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="F154" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G154" s="3" t="s">
-        <v>10</v>
+        <v>428</v>
       </c>
       <c r="H154" s="3" t="s">
         <v>131</v>
@@ -5431,13 +5521,13 @@
     </row>
     <row r="155" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C155" s="3" t="s">
-        <v>392</v>
+        <v>281</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>393</v>
+        <v>282</v>
       </c>
       <c r="E155" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F155" s="3" t="s">
         <v>9</v>
@@ -5451,13 +5541,13 @@
     </row>
     <row r="156" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C156" s="3" t="s">
-        <v>396</v>
+        <v>277</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>397</v>
+        <v>278</v>
       </c>
       <c r="E156" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F156" s="3" t="s">
         <v>9</v>
@@ -5471,13 +5561,13 @@
     </row>
     <row r="157" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C157" s="3" t="s">
-        <v>400</v>
+        <v>273</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>401</v>
+        <v>274</v>
       </c>
       <c r="E157" s="3" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="F157" s="3" t="s">
         <v>9</v>
@@ -5491,13 +5581,13 @@
     </row>
     <row r="158" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C158" s="3" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="E158" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F158" s="3" t="s">
         <v>9</v>
@@ -5511,13 +5601,13 @@
     </row>
     <row r="159" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C159" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E159" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F159" s="3" t="s">
         <v>9</v>
@@ -5531,13 +5621,13 @@
     </row>
     <row r="160" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C160" s="3" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="E160" s="3" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="F160" s="3" t="s">
         <v>9</v>
@@ -5551,13 +5641,13 @@
     </row>
     <row r="161" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C161" s="3" t="s">
-        <v>295</v>
+        <v>390</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>296</v>
+        <v>391</v>
       </c>
       <c r="E161" s="3" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="F161" s="3" t="s">
         <v>9</v>
@@ -5571,13 +5661,13 @@
     </row>
     <row r="162" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C162" s="3" t="s">
-        <v>293</v>
+        <v>386</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>294</v>
+        <v>387</v>
       </c>
       <c r="E162" s="3" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="F162" s="3" t="s">
         <v>9</v>
@@ -5591,13 +5681,13 @@
     </row>
     <row r="163" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C163" s="3" t="s">
-        <v>84</v>
+        <v>388</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>85</v>
+        <v>389</v>
       </c>
       <c r="E163" s="3" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="F163" s="3" t="s">
         <v>9</v>
@@ -5606,24 +5696,24 @@
         <v>10</v>
       </c>
       <c r="H163" s="3" t="s">
-        <v>86</v>
+        <v>131</v>
       </c>
     </row>
     <row r="164" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C164" s="3" t="s">
-        <v>429</v>
+        <v>398</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>430</v>
+        <v>399</v>
       </c>
       <c r="E164" s="3" t="s">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="F164" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G164" s="3" t="s">
-        <v>428</v>
+        <v>10</v>
       </c>
       <c r="H164" s="3" t="s">
         <v>131</v>
@@ -5631,10 +5721,10 @@
     </row>
     <row r="165" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C165" s="3" t="s">
-        <v>470</v>
+        <v>394</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>470</v>
+        <v>395</v>
       </c>
       <c r="E165" s="3" t="s">
         <v>32</v>
@@ -5643,7 +5733,7 @@
         <v>9</v>
       </c>
       <c r="G165" s="3" t="s">
-        <v>428</v>
+        <v>10</v>
       </c>
       <c r="H165" s="3" t="s">
         <v>131</v>
@@ -5651,10 +5741,10 @@
     </row>
     <row r="166" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C166" s="3" t="s">
-        <v>133</v>
+        <v>392</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>134</v>
+        <v>393</v>
       </c>
       <c r="E166" s="3" t="s">
         <v>32</v>
@@ -5671,13 +5761,13 @@
     </row>
     <row r="167" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C167" s="3" t="s">
-        <v>416</v>
+        <v>396</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>417</v>
+        <v>397</v>
       </c>
       <c r="E167" s="3" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="F167" s="3" t="s">
         <v>9</v>
@@ -5691,10 +5781,10 @@
     </row>
     <row r="168" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C168" s="3" t="s">
-        <v>414</v>
+        <v>400</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>415</v>
+        <v>401</v>
       </c>
       <c r="E168" s="3" t="s">
         <v>47</v>
@@ -5711,10 +5801,10 @@
     </row>
     <row r="169" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C169" s="3" t="s">
-        <v>412</v>
+        <v>269</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>413</v>
+        <v>270</v>
       </c>
       <c r="E169" s="3" t="s">
         <v>32</v>
@@ -5731,19 +5821,19 @@
     </row>
     <row r="170" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C170" s="3" t="s">
-        <v>473</v>
+        <v>267</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>474</v>
+        <v>268</v>
       </c>
       <c r="E170" s="3" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="F170" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G170" s="3" t="s">
-        <v>428</v>
+        <v>10</v>
       </c>
       <c r="H170" s="3" t="s">
         <v>131</v>
@@ -5751,19 +5841,19 @@
     </row>
     <row r="171" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C171" s="3" t="s">
-        <v>475</v>
+        <v>279</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>475</v>
+        <v>280</v>
       </c>
       <c r="E171" s="3" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="F171" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G171" s="3" t="s">
-        <v>428</v>
+        <v>10</v>
       </c>
       <c r="H171" s="3" t="s">
         <v>131</v>
@@ -5771,13 +5861,13 @@
     </row>
     <row r="172" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C172" s="3" t="s">
-        <v>424</v>
+        <v>295</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>424</v>
+        <v>296</v>
       </c>
       <c r="E172" s="3" t="s">
-        <v>424</v>
+        <v>23</v>
       </c>
       <c r="F172" s="3" t="s">
         <v>9</v>
@@ -5786,24 +5876,24 @@
         <v>10</v>
       </c>
       <c r="H172" s="3" t="s">
-        <v>423</v>
+        <v>131</v>
       </c>
     </row>
     <row r="173" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C173" s="3" t="s">
-        <v>463</v>
+        <v>293</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>464</v>
+        <v>294</v>
       </c>
       <c r="E173" s="3" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="F173" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G173" s="3" t="s">
-        <v>428</v>
+        <v>10</v>
       </c>
       <c r="H173" s="3" t="s">
         <v>131</v>
@@ -5811,10 +5901,10 @@
     </row>
     <row r="174" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C174" s="3" t="s">
-        <v>354</v>
+        <v>84</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>355</v>
+        <v>85</v>
       </c>
       <c r="E174" s="3" t="s">
         <v>23</v>
@@ -5826,24 +5916,24 @@
         <v>10</v>
       </c>
       <c r="H174" s="3" t="s">
-        <v>131</v>
+        <v>86</v>
       </c>
     </row>
     <row r="175" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C175" s="3" t="s">
-        <v>285</v>
+        <v>429</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>286</v>
+        <v>430</v>
       </c>
       <c r="E175" s="3" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="F175" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G175" s="3" t="s">
-        <v>10</v>
+        <v>428</v>
       </c>
       <c r="H175" s="3" t="s">
         <v>131</v>
@@ -5851,19 +5941,19 @@
     </row>
     <row r="176" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C176" s="3" t="s">
-        <v>287</v>
+        <v>470</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>288</v>
+        <v>470</v>
       </c>
       <c r="E176" s="3" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="F176" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G176" s="3" t="s">
-        <v>10</v>
+        <v>428</v>
       </c>
       <c r="H176" s="3" t="s">
         <v>131</v>
@@ -5871,13 +5961,13 @@
     </row>
     <row r="177" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C177" s="3" t="s">
-        <v>289</v>
+        <v>133</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>290</v>
+        <v>134</v>
       </c>
       <c r="E177" s="3" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="F177" s="3" t="s">
         <v>9</v>
@@ -5891,10 +5981,10 @@
     </row>
     <row r="178" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C178" s="3" t="s">
-        <v>356</v>
+        <v>416</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>357</v>
+        <v>417</v>
       </c>
       <c r="E178" s="3" t="s">
         <v>23</v>
@@ -5911,13 +6001,13 @@
     </row>
     <row r="179" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C179" s="3" t="s">
-        <v>283</v>
+        <v>414</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>284</v>
+        <v>415</v>
       </c>
       <c r="E179" s="3" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="F179" s="3" t="s">
         <v>9</v>
@@ -5931,13 +6021,13 @@
     </row>
     <row r="180" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C180" s="3" t="s">
-        <v>320</v>
+        <v>412</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>321</v>
+        <v>413</v>
       </c>
       <c r="E180" s="3" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="F180" s="3" t="s">
         <v>9</v>
@@ -5951,19 +6041,19 @@
     </row>
     <row r="181" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C181" s="3" t="s">
-        <v>263</v>
+        <v>473</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>264</v>
+        <v>474</v>
       </c>
       <c r="E181" s="3" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="F181" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G181" s="3" t="s">
-        <v>10</v>
+        <v>428</v>
       </c>
       <c r="H181" s="3" t="s">
         <v>131</v>
@@ -5971,76 +6061,76 @@
     </row>
     <row r="182" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C182" s="3" t="s">
-        <v>87</v>
+        <v>475</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>88</v>
+        <v>475</v>
       </c>
       <c r="E182" s="3" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="F182" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G182" s="3" t="s">
-        <v>10</v>
+        <v>428</v>
       </c>
       <c r="H182" s="3" t="s">
-        <v>89</v>
+        <v>131</v>
       </c>
     </row>
     <row r="183" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C183" s="3" t="s">
-        <v>249</v>
+        <v>424</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>250</v>
+        <v>424</v>
       </c>
       <c r="E183" s="3" t="s">
-        <v>247</v>
+        <v>424</v>
       </c>
       <c r="F183" s="3" t="s">
-        <v>248</v>
+        <v>9</v>
       </c>
       <c r="G183" s="3" t="s">
         <v>10</v>
       </c>
       <c r="H183" s="3" t="s">
-        <v>131</v>
+        <v>423</v>
       </c>
     </row>
     <row r="184" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C184" s="3" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E184" s="3" t="s">
-        <v>465</v>
+        <v>47</v>
       </c>
       <c r="F184" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G184" s="3" t="s">
-        <v>10</v>
+        <v>428</v>
       </c>
       <c r="H184" s="3" t="s">
-        <v>423</v>
+        <v>131</v>
       </c>
     </row>
     <row r="185" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C185" s="3" t="s">
-        <v>245</v>
+        <v>354</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>246</v>
+        <v>355</v>
       </c>
       <c r="E185" s="3" t="s">
-        <v>247</v>
+        <v>23</v>
       </c>
       <c r="F185" s="3" t="s">
-        <v>248</v>
+        <v>9</v>
       </c>
       <c r="G185" s="3" t="s">
         <v>10</v>
@@ -6051,19 +6141,19 @@
     </row>
     <row r="186" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C186" s="3" t="s">
-        <v>448</v>
+        <v>285</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>448</v>
+        <v>286</v>
       </c>
       <c r="E186" s="3" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="F186" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G186" s="3" t="s">
-        <v>428</v>
+        <v>10</v>
       </c>
       <c r="H186" s="3" t="s">
         <v>131</v>
@@ -6071,10 +6161,10 @@
     </row>
     <row r="187" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C187" s="3" t="s">
-        <v>451</v>
+        <v>287</v>
       </c>
       <c r="D187" s="3" t="s">
-        <v>451</v>
+        <v>288</v>
       </c>
       <c r="E187" s="3" t="s">
         <v>47</v>
@@ -6083,7 +6173,7 @@
         <v>9</v>
       </c>
       <c r="G187" s="3" t="s">
-        <v>428</v>
+        <v>10</v>
       </c>
       <c r="H187" s="3" t="s">
         <v>131</v>
@@ -6091,10 +6181,10 @@
     </row>
     <row r="188" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C188" s="3" t="s">
-        <v>476</v>
+        <v>289</v>
       </c>
       <c r="D188" s="3" t="s">
-        <v>476</v>
+        <v>290</v>
       </c>
       <c r="E188" s="3" t="s">
         <v>23</v>
@@ -6103,7 +6193,7 @@
         <v>9</v>
       </c>
       <c r="G188" s="3" t="s">
-        <v>428</v>
+        <v>10</v>
       </c>
       <c r="H188" s="3" t="s">
         <v>131</v>
@@ -6111,10 +6201,10 @@
     </row>
     <row r="189" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C189" s="3" t="s">
-        <v>100</v>
+        <v>356</v>
       </c>
       <c r="D189" s="3" t="s">
-        <v>101</v>
+        <v>357</v>
       </c>
       <c r="E189" s="3" t="s">
         <v>23</v>
@@ -6126,24 +6216,24 @@
         <v>10</v>
       </c>
       <c r="H189" s="3" t="s">
-        <v>102</v>
+        <v>131</v>
       </c>
     </row>
     <row r="190" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C190" s="3" t="s">
-        <v>454</v>
+        <v>283</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>455</v>
+        <v>284</v>
       </c>
       <c r="E190" s="3" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="F190" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G190" s="3" t="s">
-        <v>428</v>
+        <v>10</v>
       </c>
       <c r="H190" s="3" t="s">
         <v>131</v>
@@ -6151,19 +6241,19 @@
     </row>
     <row r="191" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C191" s="3" t="s">
-        <v>456</v>
+        <v>320</v>
       </c>
       <c r="D191" s="3" t="s">
-        <v>457</v>
+        <v>321</v>
       </c>
       <c r="E191" s="3" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="F191" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G191" s="3" t="s">
-        <v>428</v>
+        <v>10</v>
       </c>
       <c r="H191" s="3" t="s">
         <v>131</v>
@@ -6171,13 +6261,13 @@
     </row>
     <row r="192" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C192" s="3" t="s">
-        <v>135</v>
+        <v>263</v>
       </c>
       <c r="D192" s="3" t="s">
-        <v>135</v>
+        <v>264</v>
       </c>
       <c r="E192" s="3" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="F192" s="3" t="s">
         <v>9</v>
@@ -6191,10 +6281,10 @@
     </row>
     <row r="193" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C193" s="3" t="s">
-        <v>468</v>
+        <v>87</v>
       </c>
       <c r="D193" s="3" t="s">
-        <v>469</v>
+        <v>88</v>
       </c>
       <c r="E193" s="3" t="s">
         <v>32</v>
@@ -6203,27 +6293,27 @@
         <v>9</v>
       </c>
       <c r="G193" s="3" t="s">
-        <v>428</v>
+        <v>10</v>
       </c>
       <c r="H193" s="3" t="s">
-        <v>131</v>
+        <v>89</v>
       </c>
     </row>
     <row r="194" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C194" s="3" t="s">
-        <v>471</v>
+        <v>249</v>
       </c>
       <c r="D194" s="3" t="s">
-        <v>472</v>
+        <v>250</v>
       </c>
       <c r="E194" s="3" t="s">
-        <v>47</v>
+        <v>247</v>
       </c>
       <c r="F194" s="3" t="s">
-        <v>9</v>
+        <v>248</v>
       </c>
       <c r="G194" s="3" t="s">
-        <v>428</v>
+        <v>10</v>
       </c>
       <c r="H194" s="3" t="s">
         <v>131</v>
@@ -6231,13 +6321,13 @@
     </row>
     <row r="195" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C195" s="3" t="s">
-        <v>218</v>
+        <v>465</v>
       </c>
       <c r="D195" s="3" t="s">
-        <v>219</v>
+        <v>465</v>
       </c>
       <c r="E195" s="3" t="s">
-        <v>23</v>
+        <v>465</v>
       </c>
       <c r="F195" s="3" t="s">
         <v>9</v>
@@ -6246,21 +6336,21 @@
         <v>10</v>
       </c>
       <c r="H195" s="3" t="s">
-        <v>131</v>
+        <v>423</v>
       </c>
     </row>
     <row r="196" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C196" s="3" t="s">
-        <v>220</v>
+        <v>245</v>
       </c>
       <c r="D196" s="3" t="s">
-        <v>221</v>
+        <v>246</v>
       </c>
       <c r="E196" s="3" t="s">
-        <v>23</v>
+        <v>247</v>
       </c>
       <c r="F196" s="3" t="s">
-        <v>9</v>
+        <v>248</v>
       </c>
       <c r="G196" s="3" t="s">
         <v>10</v>
@@ -6271,19 +6361,19 @@
     </row>
     <row r="197" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C197" s="3" t="s">
-        <v>222</v>
+        <v>448</v>
       </c>
       <c r="D197" s="3" t="s">
-        <v>223</v>
+        <v>448</v>
       </c>
       <c r="E197" s="3" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="F197" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G197" s="3" t="s">
-        <v>10</v>
+        <v>428</v>
       </c>
       <c r="H197" s="3" t="s">
         <v>131</v>
@@ -6291,19 +6381,19 @@
     </row>
     <row r="198" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C198" s="3" t="s">
-        <v>224</v>
+        <v>451</v>
       </c>
       <c r="D198" s="3" t="s">
-        <v>225</v>
+        <v>451</v>
       </c>
       <c r="E198" s="3" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="F198" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G198" s="3" t="s">
-        <v>10</v>
+        <v>428</v>
       </c>
       <c r="H198" s="3" t="s">
         <v>131</v>
@@ -6311,10 +6401,10 @@
     </row>
     <row r="199" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C199" s="3" t="s">
-        <v>226</v>
+        <v>476</v>
       </c>
       <c r="D199" s="3" t="s">
-        <v>227</v>
+        <v>476</v>
       </c>
       <c r="E199" s="3" t="s">
         <v>23</v>
@@ -6323,7 +6413,7 @@
         <v>9</v>
       </c>
       <c r="G199" s="3" t="s">
-        <v>10</v>
+        <v>428</v>
       </c>
       <c r="H199" s="3" t="s">
         <v>131</v>
@@ -6331,39 +6421,39 @@
     </row>
     <row r="200" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C200" s="3" t="s">
-        <v>466</v>
+        <v>100</v>
       </c>
       <c r="D200" s="3" t="s">
-        <v>467</v>
+        <v>101</v>
       </c>
       <c r="E200" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F200" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G200" s="3" t="s">
-        <v>428</v>
+        <v>10</v>
       </c>
       <c r="H200" s="3" t="s">
-        <v>131</v>
+        <v>102</v>
       </c>
     </row>
     <row r="201" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C201" s="3" t="s">
-        <v>420</v>
+        <v>454</v>
       </c>
       <c r="D201" s="3" t="s">
-        <v>421</v>
+        <v>455</v>
       </c>
       <c r="E201" s="3" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="F201" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G201" s="3" t="s">
-        <v>10</v>
+        <v>428</v>
       </c>
       <c r="H201" s="3" t="s">
         <v>131</v>
@@ -6371,33 +6461,33 @@
     </row>
     <row r="202" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C202" s="3" t="s">
-        <v>329</v>
+        <v>456</v>
       </c>
       <c r="D202" s="3" t="s">
-        <v>330</v>
+        <v>457</v>
       </c>
       <c r="E202" s="3" t="s">
-        <v>111</v>
+        <v>47</v>
       </c>
       <c r="F202" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G202" s="3" t="s">
-        <v>10</v>
+        <v>428</v>
       </c>
       <c r="H202" s="3" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
     </row>
     <row r="203" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C203" s="3" t="s">
-        <v>327</v>
+        <v>135</v>
       </c>
       <c r="D203" s="3" t="s">
-        <v>328</v>
+        <v>135</v>
       </c>
       <c r="E203" s="3" t="s">
-        <v>111</v>
+        <v>23</v>
       </c>
       <c r="F203" s="3" t="s">
         <v>9</v>
@@ -6406,78 +6496,78 @@
         <v>10</v>
       </c>
       <c r="H203" s="3" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
     </row>
     <row r="204" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C204" s="3" t="s">
-        <v>337</v>
+        <v>468</v>
       </c>
       <c r="D204" s="3" t="s">
-        <v>338</v>
+        <v>469</v>
       </c>
       <c r="E204" s="3" t="s">
-        <v>111</v>
+        <v>32</v>
       </c>
       <c r="F204" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G204" s="3" t="s">
-        <v>10</v>
+        <v>428</v>
       </c>
       <c r="H204" s="3" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
     </row>
     <row r="205" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C205" s="3" t="s">
-        <v>335</v>
+        <v>471</v>
       </c>
       <c r="D205" s="3" t="s">
-        <v>336</v>
+        <v>472</v>
       </c>
       <c r="E205" s="3" t="s">
-        <v>111</v>
+        <v>47</v>
       </c>
       <c r="F205" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G205" s="3" t="s">
-        <v>10</v>
+        <v>428</v>
       </c>
       <c r="H205" s="3" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
     </row>
     <row r="206" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C206" s="3" t="s">
-        <v>333</v>
+        <v>466</v>
       </c>
       <c r="D206" s="3" t="s">
-        <v>334</v>
+        <v>467</v>
       </c>
       <c r="E206" s="3" t="s">
-        <v>111</v>
+        <v>32</v>
       </c>
       <c r="F206" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G206" s="3" t="s">
-        <v>10</v>
+        <v>428</v>
       </c>
       <c r="H206" s="3" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
     </row>
     <row r="207" spans="3:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C207" s="3" t="s">
-        <v>325</v>
+        <v>420</v>
       </c>
       <c r="D207" s="3" t="s">
-        <v>326</v>
+        <v>421</v>
       </c>
       <c r="E207" s="3" t="s">
-        <v>111</v>
+        <v>32</v>
       </c>
       <c r="F207" s="3" t="s">
         <v>9</v>
@@ -6486,7 +6576,7 @@
         <v>10</v>
       </c>
       <c r="H207" s="3" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
     </row>
     <row r="208" spans="3:8" ht="19" x14ac:dyDescent="0.25">
@@ -6930,9 +7020,9 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H229">
-    <sortCondition ref="A2:A229"/>
-    <sortCondition ref="B2:B229"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H231">
+    <sortCondition ref="A2:A231"/>
+    <sortCondition ref="B2:B231"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>